<commit_message>
super scheduler mostly completed
Performed bulk of work on superplayoff scheduler. Renamed everything from Sunday to "super" to represent superplayoffs. Super_input now correctly orders brackets based on top finish order, not alphabetically by bracket name.
</commit_message>
<xml_diff>
--- a/inputs/prelim_results.xlsx
+++ b/inputs/prelim_results.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/victorprieto/Desktop/code/cornerstone/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F08DFE0B-B243-4243-BC35-E445E0F19EAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96D285E2-243F-9F47-A02F-4C99989E8A89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2660" yWindow="1560" windowWidth="28260" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1190,8 +1190,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20"/>

</xml_diff>